<commit_message>
fix: parent updating when eft changes in network
</commit_message>
<xml_diff>
--- a/apps/explorer/src/assets/sample-data/project-network.xlsx
+++ b/apps/explorer/src/assets/sample-data/project-network.xlsx
@@ -7,12 +7,15 @@
     <sheet name="Arrow Info" sheetId="2" r:id="rId2"/>
     <sheet name="Integrations" sheetId="3" r:id="rId3"/>
     <sheet name="Profile" sheetId="4" r:id="rId4"/>
-    <sheet name="Phases" sheetId="5" r:id="rId5"/>
-    <sheet name="Roles" sheetId="6" r:id="rId6"/>
-    <sheet name="Resources" sheetId="7" r:id="rId7"/>
-    <sheet name="Activity Assigned Resources" sheetId="8" r:id="rId8"/>
-    <sheet name="Activity Assinged Phases" sheetId="9" r:id="rId9"/>
-    <sheet name="Resource Roles" sheetId="10" r:id="rId10"/>
+    <sheet name="Sub-Parent Projects" sheetId="5" r:id="rId5"/>
+    <sheet name="Phases" sheetId="6" r:id="rId6"/>
+    <sheet name="Roles" sheetId="7" r:id="rId7"/>
+    <sheet name="Resources" sheetId="8" r:id="rId8"/>
+    <sheet name="Activity Assigned Resources" sheetId="9" r:id="rId9"/>
+    <sheet name="Activity Assinged Phases" sheetId="10" r:id="rId10"/>
+    <sheet name="Resource Roles" sheetId="11" r:id="rId11"/>
+    <sheet name="Tag Pool" sheetId="12" r:id="rId12"/>
+    <sheet name="Activity Tags" sheetId="13" r:id="rId13"/>
   </sheets>
 </workbook>
 </file>
@@ -16973,6 +16976,19 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17137,6 +17153,32 @@
   </sheetData>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:F9"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -17401,7 +17443,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>7</v>
@@ -23367,7 +23409,7 @@
         <v>0</v>
       </c>
       <c r="I195" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K195">
         <v>2</v>
@@ -23399,7 +23441,7 @@
         <v>0</v>
       </c>
       <c r="I196" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K196">
         <v>3</v>
@@ -25127,7 +25169,7 @@
         <v>0</v>
       </c>
       <c r="I250" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K250">
         <v>7</v>
@@ -25621,7 +25663,7 @@
         <v>0</v>
       </c>
       <c r="I266" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K266">
         <v>6</v>
@@ -30981,7 +31023,7 @@
         <v>874</v>
       </c>
       <c r="R10" t="str">
-        <v>4/28/2016</v>
+        <v>4/14/2016</v>
       </c>
       <c r="S10" t="b">
         <v>0</v>
@@ -31158,7 +31200,7 @@
         <v>874</v>
       </c>
       <c r="R13" t="str">
-        <v>5/30/2016</v>
+        <v>4/7/2016</v>
       </c>
       <c r="S13" t="b">
         <v>0</v>
@@ -31276,7 +31318,7 @@
         <v>874</v>
       </c>
       <c r="R15" t="str">
-        <v>5/30/2016</v>
+        <v>4/13/2016</v>
       </c>
       <c r="S15" t="b">
         <v>0</v>
@@ -31453,7 +31495,7 @@
         <v>1538</v>
       </c>
       <c r="R18" t="str">
-        <v>7/19/2016</v>
+        <v>4/20/2016</v>
       </c>
       <c r="S18" t="b">
         <v>1</v>
@@ -32161,7 +32203,7 @@
         <v>70</v>
       </c>
       <c r="R30" t="str">
-        <v>5/16/2016</v>
+        <v>3/22/2016</v>
       </c>
       <c r="S30" t="b">
         <v>0</v>
@@ -32515,7 +32557,7 @@
         <v>135</v>
       </c>
       <c r="R36" t="str">
-        <v>7/10/2016</v>
+        <v>4/28/2016</v>
       </c>
       <c r="S36" t="b">
         <v>0</v>
@@ -32987,7 +33029,7 @@
         <v>590</v>
       </c>
       <c r="R44" t="str">
-        <v>10/22/2016</v>
+        <v>10/18/2016</v>
       </c>
       <c r="S44" t="b">
         <v>0</v>
@@ -33105,7 +33147,7 @@
         <v>640</v>
       </c>
       <c r="R46" t="str">
-        <v>11/5/2016</v>
+        <v>11/3/2016</v>
       </c>
       <c r="S46" t="b">
         <v>0</v>
@@ -33164,7 +33206,7 @@
         <v>644</v>
       </c>
       <c r="R47" t="str">
-        <v>11/5/2016</v>
+        <v>11/3/2016</v>
       </c>
       <c r="S47" t="b">
         <v>0</v>
@@ -33223,7 +33265,7 @@
         <v>650</v>
       </c>
       <c r="R48" t="str">
-        <v>11/15/2016</v>
+        <v>11/13/2016</v>
       </c>
       <c r="S48" t="b">
         <v>0</v>
@@ -33282,7 +33324,7 @@
         <v>654</v>
       </c>
       <c r="R49" t="str">
-        <v>11/19/2016</v>
+        <v>11/17/2016</v>
       </c>
       <c r="S49" t="b">
         <v>0</v>
@@ -36232,7 +36274,7 @@
         <v>30</v>
       </c>
       <c r="R99" t="str">
-        <v>2/13/2015</v>
+        <v>1/23/2015</v>
       </c>
       <c r="S99" t="b">
         <v>0</v>
@@ -36822,7 +36864,7 @@
         <v>55</v>
       </c>
       <c r="R109" t="str">
-        <v>3/6/2015</v>
+        <v>2/27/2015</v>
       </c>
       <c r="S109" t="b">
         <v>0</v>
@@ -37235,7 +37277,7 @@
         <v>85</v>
       </c>
       <c r="R116" t="str">
-        <v>4/3/2015</v>
+        <v>3/20/2015</v>
       </c>
       <c r="S116" t="b">
         <v>0</v>
@@ -37353,7 +37395,7 @@
         <v>210</v>
       </c>
       <c r="R118" t="str">
-        <v>4/10/2015</v>
+        <v>4/3/2015</v>
       </c>
       <c r="S118" t="b">
         <v>0</v>
@@ -37412,7 +37454,7 @@
         <v>95</v>
       </c>
       <c r="R119" t="str">
-        <v>4/24/2015</v>
+        <v>4/10/2015</v>
       </c>
       <c r="S119" t="b">
         <v>0</v>
@@ -37648,7 +37690,7 @@
         <v>135</v>
       </c>
       <c r="R123" t="str">
-        <v>6/5/2015</v>
+        <v>5/8/2015</v>
       </c>
       <c r="S123" t="b">
         <v>0</v>
@@ -38297,7 +38339,7 @@
         <v>235</v>
       </c>
       <c r="R134" t="str">
-        <v>11/6/2015</v>
+        <v>10/30/2015</v>
       </c>
       <c r="S134" t="b">
         <v>0</v>
@@ -38474,7 +38516,7 @@
         <v>245</v>
       </c>
       <c r="R137" t="str">
-        <v>11/20/2015</v>
+        <v>5/29/2015</v>
       </c>
       <c r="S137" t="b">
         <v>0</v>
@@ -40539,7 +40581,7 @@
         <v>95</v>
       </c>
       <c r="R172" t="str">
-        <v>6/7/2013</v>
+        <v>4/26/2013</v>
       </c>
       <c r="S172" t="b">
         <v>0</v>
@@ -40657,7 +40699,7 @@
         <v>95</v>
       </c>
       <c r="R174" t="str">
-        <v>6/7/2013</v>
+        <v>5/31/2013</v>
       </c>
       <c r="S174" t="b">
         <v>0</v>
@@ -40834,7 +40876,7 @@
         <v>115</v>
       </c>
       <c r="R177" t="str">
-        <v>7/12/2013</v>
+        <v>7/5/2013</v>
       </c>
       <c r="S177" t="b">
         <v>0</v>
@@ -40893,7 +40935,7 @@
         <v>130</v>
       </c>
       <c r="R178" t="str">
-        <v>8/9/2013</v>
+        <v>7/12/2013</v>
       </c>
       <c r="S178" t="b">
         <v>0</v>
@@ -41778,7 +41820,7 @@
         <v>95</v>
       </c>
       <c r="R193" t="str">
-        <v>5/10/2013</v>
+        <v>4/26/2013</v>
       </c>
       <c r="S193" t="b">
         <v>0</v>
@@ -41837,7 +41879,7 @@
         <v>100</v>
       </c>
       <c r="R194" t="str">
-        <v>5/10/2013</v>
+        <v>4/26/2013</v>
       </c>
       <c r="S194" t="b">
         <v>0</v>
@@ -41955,7 +41997,7 @@
         <v>115</v>
       </c>
       <c r="R196" t="str">
-        <v>6/7/2013</v>
+        <v>5/31/2013</v>
       </c>
       <c r="S196" t="b">
         <v>0</v>
@@ -42014,7 +42056,7 @@
         <v>120</v>
       </c>
       <c r="R197" t="str">
-        <v>6/21/2013</v>
+        <v>5/31/2013</v>
       </c>
       <c r="S197" t="b">
         <v>0</v>
@@ -42073,7 +42115,7 @@
         <v>135</v>
       </c>
       <c r="R198" t="str">
-        <v>7/12/2013</v>
+        <v>5/31/2013</v>
       </c>
       <c r="S198" t="b">
         <v>0</v>
@@ -42191,7 +42233,7 @@
         <v>135</v>
       </c>
       <c r="R200" t="str">
-        <v>7/5/2013</v>
+        <v>5/31/2013</v>
       </c>
       <c r="S200" t="b">
         <v>0</v>
@@ -42250,7 +42292,7 @@
         <v>140</v>
       </c>
       <c r="R201" t="str">
-        <v>7/19/2013</v>
+        <v>7/12/2013</v>
       </c>
       <c r="S201" t="b">
         <v>0</v>
@@ -46911,7 +46953,7 @@
         <v>80</v>
       </c>
       <c r="R280" t="str">
-        <v>3/15/2021</v>
+        <v>3/8/2021</v>
       </c>
       <c r="S280" t="b">
         <v>0</v>
@@ -47345,7 +47387,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -47414,6 +47456,9 @@
       <c r="U1" t="str">
         <v>nodeId</v>
       </c>
+      <c r="V1" t="str">
+        <v>parentProjectId</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -47502,6 +47547,9 @@
       <c r="U3">
         <v>1797</v>
       </c>
+      <c r="V3">
+        <v>720</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -47546,6 +47594,9 @@
       <c r="U4">
         <v>1890</v>
       </c>
+      <c r="V4">
+        <v>720</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -47590,6 +47641,9 @@
       <c r="U5">
         <v>3712</v>
       </c>
+      <c r="V5">
+        <v>720</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -47634,6 +47688,9 @@
       <c r="U6">
         <v>91</v>
       </c>
+      <c r="V6">
+        <v>720</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -47678,6 +47735,9 @@
       <c r="U7">
         <v>155</v>
       </c>
+      <c r="V7">
+        <v>1797</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -47722,6 +47782,9 @@
       <c r="U8">
         <v>421</v>
       </c>
+      <c r="V8">
+        <v>1797</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -47766,6 +47829,9 @@
       <c r="U9">
         <v>469</v>
       </c>
+      <c r="V9">
+        <v>421</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -47810,6 +47876,9 @@
       <c r="U10">
         <v>1142</v>
       </c>
+      <c r="V10">
+        <v>421</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -47853,6 +47922,9 @@
       </c>
       <c r="U11">
         <v>1360</v>
+      </c>
+      <c r="V11">
+        <v>1142</v>
       </c>
     </row>
     <row r="12">
@@ -47898,15 +47970,269 @@
       <c r="U12">
         <v>1550</v>
       </c>
+      <c r="V12">
+        <v>1142</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:U12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:V12"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>clearSelectedArrow</v>
+      </c>
+      <c r="B1" t="str">
+        <v>activityParentId</v>
+      </c>
+      <c r="C1" t="str">
+        <v>riskDepthCalc</v>
+      </c>
+      <c r="D1" t="str">
+        <v>activityParentName</v>
+      </c>
+      <c r="E1" t="str">
+        <v>graphId</v>
+      </c>
+      <c r="F1" t="str">
+        <v>nodeId</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <v>top-level</v>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2">
+        <v>720</v>
+      </c>
+      <c r="F2">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="str">
+        <v>top-level</v>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3">
+        <v>1797</v>
+      </c>
+      <c r="F3">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="str">
+        <v>top-level</v>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4">
+        <v>1890</v>
+      </c>
+      <c r="F4">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="str">
+        <v>top-level</v>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+      <c r="E5">
+        <v>3712</v>
+      </c>
+      <c r="F5">
+        <v>3712</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6" t="str">
+        <v>top-level</v>
+      </c>
+      <c r="D6" t="str">
+        <v/>
+      </c>
+      <c r="E6">
+        <v>91</v>
+      </c>
+      <c r="F6">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="str">
+        <v>top-level</v>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+      <c r="E7">
+        <v>155</v>
+      </c>
+      <c r="F7">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="str">
+        <v>top-level</v>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
+      <c r="E8">
+        <v>421</v>
+      </c>
+      <c r="F8">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="str">
+        <v>top-level</v>
+      </c>
+      <c r="D9" t="str">
+        <v/>
+      </c>
+      <c r="E9">
+        <v>469</v>
+      </c>
+      <c r="F9">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="str">
+        <v>top-level</v>
+      </c>
+      <c r="D10" t="str">
+        <v/>
+      </c>
+      <c r="E10">
+        <v>1142</v>
+      </c>
+      <c r="F10">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="str">
+        <v>top-level</v>
+      </c>
+      <c r="D11" t="str">
+        <v/>
+      </c>
+      <c r="E11">
+        <v>1360</v>
+      </c>
+      <c r="F11">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="str">
+        <v>top-level</v>
+      </c>
+      <c r="D12" t="str">
+        <v/>
+      </c>
+      <c r="E12">
+        <v>1550</v>
+      </c>
+      <c r="F12">
+        <v>1550</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:F12"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -48079,7 +48405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -48110,12 +48436,6 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>Tester</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
       <c r="F2">
         <v>720</v>
       </c>
@@ -48124,12 +48444,6 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
-        <v>Project Manager</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
       <c r="F3">
         <v>720</v>
       </c>
@@ -48138,12 +48452,6 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
-        <v>Software Developer</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
       <c r="F4">
         <v>720</v>
       </c>
@@ -48152,12 +48460,6 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
-        <v>Architect</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
-      </c>
       <c r="F5">
         <v>720</v>
       </c>
@@ -48172,7 +48474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S8"/>
   <sheetViews>
@@ -48658,7 +48960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J22"/>
   <sheetViews>
@@ -49311,17 +49613,4 @@
     <ignoredError numberStoredAsText="1" sqref="A1:J22"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>